<commit_message>
Updated statistics and added graphs for the presentation
</commit_message>
<xml_diff>
--- a/Presentation/Performance Comparison Charts.xlsx
+++ b/Presentation/Performance Comparison Charts.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spf/Library/Mobile Documents/com~apple~CloudDocs/College/Junior year/Spring 2018/Robotics/E160-Final-Project/Presentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Hill/Documents/School/Senior/Spring/E160/E160-Final-Project/Presentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95189EDE-D2F2-424F-9440-CEEA7030EF81}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C049AA32-94D4-6346-9FAA-5C6ED060CF37}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{CFBCA617-26EF-9B42-A5E7-A705E1A357AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>Path Distance</t>
   </si>
@@ -65,12 +65,36 @@
   <si>
     <t>nodes</t>
   </si>
+  <si>
+    <t>BFS Time STDEV</t>
+  </si>
+  <si>
+    <t>BFS Nodes</t>
+  </si>
+  <si>
+    <t>BFS Nodes STDEV</t>
+  </si>
+  <si>
+    <t>aStar Time STDEV</t>
+  </si>
+  <si>
+    <t>aStar Nodes</t>
+  </si>
+  <si>
+    <t>aStar Nodes STDEV</t>
+  </si>
+  <si>
+    <t>Diff Times</t>
+  </si>
+  <si>
+    <t>Diff Nodes</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -82,6 +106,12 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF454545"/>
+      <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -105,10 +135,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1132,6 +1164,1305 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2160" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Algorithm Speed Comparison</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2160" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.16605218264437829"/>
+          <c:y val="0.13321016779517347"/>
+          <c:w val="0.78994974359499792"/>
+          <c:h val="0.76891632709335456"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BFS Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$R$2:$R$5</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>3.6399999999999997E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2.969293001E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3.1001392509999999E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>3.9528556579999999E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$R$2:$R$5</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>3.6399999999999997E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2.969293001E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3.1001392509999999E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>3.9528556579999999E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$P$2:$P$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$Q$2:$Q$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0" formatCode="0.00E+00">
+                  <c:v>9.3599999999999998E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.1966171259999997E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.2428379060000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.7156507969999996E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B9F5-A948-B3FB-C94EFC35E821}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$U$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>aStar Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$V$2:$V$5</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>5.8300000000000001E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>4.2124399570000001E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>4.6725430400000002E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>5.3693784979999999E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$V$2:$V$5</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>5.8300000000000001E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>4.2124399570000001E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>4.6725430400000002E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>5.3693784979999999E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$P$2:$P$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$U$2:$U$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.0704517360000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.801032066E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.4907121660000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.7489004139999998E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-B9F5-A948-B3FB-C94EFC35E821}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1591944095"/>
+        <c:axId val="1591942687"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1591944095"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="11000"/>
+          <c:min val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Nodes in Graph</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.31226973498839644"/>
+              <c:y val="0.90990859605584318"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1591942687"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1591942687"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Mean Time to Completion (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1591944095"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.66969933247608837"/>
+          <c:y val="0.91503191478497092"/>
+          <c:w val="0.28682345084488231"/>
+          <c:h val="7.3659442284524951E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2160" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>aStar Compared</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> to BFS</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2160" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AA$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Diff Nodes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$AB:$AB</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1048576"/>
+                  <c:pt idx="1">
+                    <c:v>1.3273658124300001</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>25.810422313499998</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>299.71756304899998</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>3280.0619325100001</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$AB:$AB</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1048576"/>
+                  <c:pt idx="1">
+                    <c:v>1.3273658124300001</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>25.810422313499998</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>299.71756304899998</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>3280.0619325100001</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$P$2:$P$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$AA$2:$AA$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>-1.0900000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-10.61</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-108.68</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-552.66999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C088-EA4E-8310-E36EBCC28869}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1628742351"/>
+        <c:axId val="1628813711"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1628742351"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="11000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Nodes in Graph</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1628813711"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1628813711"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Relative</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Difference in Nodes</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1628742351"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1212,6 +2543,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -1716,6 +3127,1038 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2300,6 +4743,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15E6E5DB-4FBE-BC42-9597-64E9AE6FB113}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>113195</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>185254</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>320261</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{787714CF-FCFE-B94C-AFAB-57038106A41E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2605,15 +5120,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D469F8F0-71DC-E344-BE4E-97C1600A9AAD}">
-  <dimension ref="A1:X5"/>
+  <dimension ref="A1:AC5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2644,14 +5159,51 @@
       <c r="P1" t="s">
         <v>12</v>
       </c>
+      <c r="Q1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U1" t="s">
+        <v>8</v>
+      </c>
+      <c r="V1" t="s">
+        <v>16</v>
+      </c>
+      <c r="W1" t="s">
+        <v>17</v>
+      </c>
+      <c r="X1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
         <v>4511</v>
       </c>
+      <c r="C2">
+        <f>B2-B3</f>
+        <v>1005</v>
+      </c>
       <c r="D2" t="s">
         <v>4</v>
       </c>
@@ -2703,14 +5255,34 @@
       <c r="X2" s="1">
         <v>1.9302590500000001</v>
       </c>
+      <c r="Y2" s="3">
+        <v>1.5077590942399999E-5</v>
+      </c>
+      <c r="Z2" s="3">
+        <v>3.1291166824699998E-5</v>
+      </c>
+      <c r="AA2" s="4">
+        <v>-1.0900000000000001</v>
+      </c>
+      <c r="AB2" s="4">
+        <v>1.3273658124300001</v>
+      </c>
+      <c r="AC2" s="4">
+        <f>-AA2</f>
+        <v>1.0900000000000001</v>
+      </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
         <v>3506</v>
       </c>
+      <c r="C3">
+        <f>(B3-B2)/B3</f>
+        <v>-0.28665145464917285</v>
+      </c>
       <c r="D3" t="s">
         <v>5</v>
       </c>
@@ -2762,8 +5334,24 @@
       <c r="X3" s="1">
         <v>25.024090390000001</v>
       </c>
+      <c r="Y3" s="3">
+        <v>5.4814815521200003E-5</v>
+      </c>
+      <c r="Z3" s="4">
+        <v>3.9056122552899998E-4</v>
+      </c>
+      <c r="AA3" s="4">
+        <v>-10.61</v>
+      </c>
+      <c r="AB3" s="4">
+        <v>25.810422313499998</v>
+      </c>
+      <c r="AC3" s="4">
+        <f t="shared" ref="AC3:AC5" si="0">-AA3</f>
+        <v>10.61</v>
+      </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="H4">
         <v>1000</v>
       </c>
@@ -2800,8 +5388,24 @@
       <c r="X4" s="1">
         <v>269.8877018</v>
       </c>
+      <c r="Y4" s="4">
+        <v>5.4926395416300005E-4</v>
+      </c>
+      <c r="Z4" s="4">
+        <v>5.2021977938099999E-3</v>
+      </c>
+      <c r="AA4" s="4">
+        <v>-108.68</v>
+      </c>
+      <c r="AB4" s="4">
+        <v>299.71756304899998</v>
+      </c>
+      <c r="AC4" s="4">
+        <f t="shared" si="0"/>
+        <v>108.68</v>
+      </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="H5">
         <v>10000</v>
       </c>
@@ -2837,6 +5441,22 @@
       </c>
       <c r="X5" s="1">
         <v>2850.8258249999999</v>
+      </c>
+      <c r="Y5" s="4">
+        <v>9.8862862587E-3</v>
+      </c>
+      <c r="Z5" s="4">
+        <v>6.1603469747300001E-2</v>
+      </c>
+      <c r="AA5" s="4">
+        <v>-552.66999999999996</v>
+      </c>
+      <c r="AB5" s="4">
+        <v>3280.0619325100001</v>
+      </c>
+      <c r="AC5" s="4">
+        <f t="shared" si="0"/>
+        <v>552.66999999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>